<commit_message>
added the real time
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/ImporterSeances.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/ImporterSeances.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>Semaine</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Module</t>
   </si>
   <si>
-    <t>S 1</t>
-  </si>
-  <si>
     <t>3.GINFO</t>
   </si>
   <si>
@@ -66,13 +63,19 @@
   </si>
   <si>
     <t>Mercredi</t>
+  </si>
+  <si>
+    <t>S 11</t>
+  </si>
+  <si>
+    <t>S 12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +86,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -107,10 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:I11"/>
+  <dimension ref="D7:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,13 +436,13 @@
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
       </c>
       <c r="G8" s="1">
         <v>0.33333333333333331</v>
@@ -441,18 +451,18 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
         <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
       </c>
       <c r="G9" s="1">
         <v>0.66666666666666663</v>
@@ -461,18 +471,18 @@
         <v>0.75</v>
       </c>
       <c r="I9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1">
         <v>0.41666666666666669</v>
@@ -481,18 +491,18 @@
         <v>0.5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1">
         <v>0.33333333333333331</v>
@@ -500,9 +510,94 @@
       <c r="H11" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
         <v>12</v>
       </c>
+      <c r="G15" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>